<commit_message>
documentation of some files updated
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\te2004b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D85457-B92F-4F77-9D89-C2BFA268BC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA3F0D9-B4D0-4F5A-AB3D-46D662E656FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18555" yWindow="990" windowWidth="19575" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13695" yWindow="1020" windowWidth="19575" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>C++</t>
   </si>
@@ -63,13 +63,25 @@
   </si>
   <si>
     <t>Threads</t>
+  </si>
+  <si>
+    <t>EVEN NUMBERS</t>
+  </si>
+  <si>
+    <t>PRIME NUMBERS</t>
+  </si>
+  <si>
+    <t>ENUMERATION</t>
+  </si>
+  <si>
+    <t>MERGE SORT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,14 +91,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -114,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -122,7 +126,6 @@
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,115 +502,183 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3" t="s">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>1</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B14" t="s">
         <v>3</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>2</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>3</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>4</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>5</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>6</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>8</v>
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
       <c r="C18" s="4"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
       <c r="C20" s="4"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
       <c r="C21" s="4"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
       <c r="C22" s="4"/>
       <c r="D22" s="1"/>
       <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="4"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="4"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="4"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
codes and speedup updated
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\te2004b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA3F0D9-B4D0-4F5A-AB3D-46D662E656FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC2E7FF-9050-40E9-B524-637923972560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13695" yWindow="1020" windowWidth="19575" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="195" windowWidth="19575" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,8 +442,12 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="1">
+        <v>20530</v>
+      </c>
+      <c r="D3" s="1">
+        <v>7343.4</v>
+      </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -453,8 +457,12 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="C4" s="1">
+        <v>12323</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3917</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -464,8 +472,12 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1">
+        <v>86954</v>
+      </c>
+      <c r="D5" s="1">
+        <v>66318</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -475,8 +487,12 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="1">
+        <v>20577</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7585.1</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -486,8 +502,12 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="1">
+        <v>1276.2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>90.274000000000001</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -497,8 +517,12 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="4">
+        <v>349.24079999999998</v>
+      </c>
+      <c r="D8" s="4">
+        <v>10573.045700000001</v>
+      </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -563,7 +587,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1">
+        <f>C3/D3</f>
+        <v>2.7957077103249177</v>
+      </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -574,7 +601,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1">
+        <f>C4/D4</f>
+        <v>3.1460301250957365</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -585,7 +615,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1">
+        <f>C5/D5</f>
+        <v>1.3111674055309268</v>
+      </c>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -596,7 +629,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1">
+        <f>C6/D6</f>
+        <v>2.7128185521614743</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -607,7 +643,10 @@
         <v>7</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1">
+        <f>C7/D7</f>
+        <v>14.136960808206128</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -618,7 +657,10 @@
         <v>8</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1">
+        <f>C8/D8</f>
+        <v>3.3031239049690284E-2</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
examples and exercises updated
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t xml:space="preserve">THREADS = 8</t>
   </si>
@@ -28,19 +28,44 @@
     <t xml:space="preserve">C/C++</t>
   </si>
   <si>
-    <t xml:space="preserve">Posix Thread</t>
+    <t xml:space="preserve">Pthreads</t>
   </si>
   <si>
     <t xml:space="preserve">OpenMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD VECTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPLACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATRIX X VECTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINIMUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROX PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTEGRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLUR IMAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MERGE SORT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -116,7 +141,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -127,17 +152,33 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -158,19 +199,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1019" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -182,10 +223,10 @@
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -193,148 +234,245 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2"/>
-      <c r="D12" s="3" t="s">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
+      <c r="A22" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
+      <c r="A23" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
+      <c r="A24" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D29" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>